<commit_message>
Changed Kill process properties to Current user. Made slight update to exception handling
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55648C\Documents\SOK_GIT\P0001_090_PayCyleQueries_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9853649B-DDBF-45D5-9C8C-8BC8B564BD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C30489A-66BB-4DE7-8D52-6D41E017713D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="167">
   <si>
     <t>Name</t>
   </si>
@@ -89,15 +89,15 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -163,9 +163,6 @@
     <t>P001_090_PayCycleQueries_SharepointURL</t>
   </si>
   <si>
-    <t>DEV</t>
-  </si>
-  <si>
     <t>PeoplesoftURL</t>
   </si>
   <si>
@@ -256,12 +253,6 @@
     <t>Exception Type</t>
   </si>
   <si>
-    <t>Bot Responsibility</t>
-  </si>
-  <si>
-    <t>Business or Support Team Responsibility</t>
-  </si>
-  <si>
     <t>Subject</t>
   </si>
   <si>
@@ -271,16 +262,10 @@
     <t>Notification Type</t>
   </si>
   <si>
-    <t>Timing of Notification</t>
-  </si>
-  <si>
     <t>To</t>
   </si>
   <si>
     <t>CC</t>
-  </si>
-  <si>
-    <t>Recovery Steps If Applicable</t>
   </si>
   <si>
     <t>Complete</t>
@@ -299,9 +284,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>End of the process</t>
-  </si>
-  <si>
     <t>Business</t>
   </si>
   <si>
@@ -311,22 +293,7 @@
     <t>SE_1</t>
   </si>
   <si>
-    <t>SE_1: PeopleSoft application unavailable</t>
-  </si>
-  <si>
     <t>System Exception</t>
-  </si>
-  <si>
-    <t>Bot:
-- Take screenshot
--  Send notification to business &amp; support team
-- Terminate</t>
-  </si>
-  <si>
-    <t>Perform the process manually</t>
-  </si>
-  <si>
-    <t>PeopleSoft application unavailable</t>
   </si>
   <si>
     <t>Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
@@ -335,19 +302,7 @@
 Automation Team</t>
   </si>
   <si>
-    <t>At the time of exception</t>
-  </si>
-  <si>
-    <t>Retry 3 times before erroring out</t>
-  </si>
-  <si>
     <t>SE_2</t>
-  </si>
-  <si>
-    <t>SE_2: PeopleSoft login failed</t>
-  </si>
-  <si>
-    <t>PeopleSoft login failed</t>
   </si>
   <si>
     <r>
@@ -385,15 +340,192 @@
     </r>
   </si>
   <si>
-    <t>SE_3</t>
-  </si>
-  <si>
-    <t>SE_3: Duration drop down does not exist</t>
+    <t>Business Exception</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>BE_5</t>
+  </si>
+  <si>
+    <t>SummaryPath</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_SummaryPath</t>
+  </si>
+  <si>
+    <t>BE_6</t>
+  </si>
+  <si>
+    <t>BE_7</t>
+  </si>
+  <si>
+    <t>BotControllerEmailID</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_BotControllerEmailID</t>
+  </si>
+  <si>
+    <t>The email IDs separated by comma for Bot controllers</t>
+  </si>
+  <si>
+    <t>BusinessEmailID</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_BusinessEmailID</t>
+  </si>
+  <si>
+    <t>The email IDs separated by comma for Business team</t>
+  </si>
+  <si>
+    <t>BotEmailID</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_BotEmailID</t>
+  </si>
+  <si>
+    <t>The email ID of the service account</t>
+  </si>
+  <si>
+    <t>DatetimeFormat</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_ProcessMonitorDatetimeFormat</t>
+  </si>
+  <si>
+    <t>The format of the date in process monitor to validate the run time of each instance</t>
+  </si>
+  <si>
+    <t>MorningStartTime</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_MorningRun_StartTime</t>
+  </si>
+  <si>
+    <t>Date time for Morning run</t>
+  </si>
+  <si>
+    <t>MorningEndTime</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_MorningRun_EndTime</t>
+  </si>
+  <si>
+    <t>NoonStartTime</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_NoonRun_StartTime</t>
+  </si>
+  <si>
+    <t>Date time for Noon run</t>
+  </si>
+  <si>
+    <t>NoonEndTime</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_NoonRun_EndTime</t>
+  </si>
+  <si>
+    <t>EveningStartTime</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_EveningRun_StartTime</t>
+  </si>
+  <si>
+    <t>Date time for Evening run</t>
+  </si>
+  <si>
+    <t>EveningEndTime</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_EveningRun_EndTime</t>
+  </si>
+  <si>
+    <t>StartEndTimeFormat</t>
+  </si>
+  <si>
+    <t>MM-dd-yyyy h:mmtt</t>
+  </si>
+  <si>
+    <t>The format used to parse time from assets</t>
+  </si>
+  <si>
+    <t>AssetFolder</t>
+  </si>
+  <si>
+    <t>TenantID</t>
+  </si>
+  <si>
+    <t>Shared_O365TenantID</t>
+  </si>
+  <si>
+    <t>Name of the Tenant ID Asset</t>
+  </si>
+  <si>
+    <t>AppID</t>
+  </si>
+  <si>
+    <t>Shared_O365ApplicationID</t>
+  </si>
+  <si>
+    <t>Name of the App ID Asset</t>
+  </si>
+  <si>
+    <t>AppSecret</t>
+  </si>
+  <si>
+    <t>Shared_O365ApplicationSecret</t>
+  </si>
+  <si>
+    <t>Name of the App Secret Asset</t>
+  </si>
+  <si>
+    <t>BE_8</t>
+  </si>
+  <si>
+    <t>SE_1:PeopleSoft application unavailable</t>
+  </si>
+  <si>
+    <t>SE_2:PeopleSoft login failed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BE_5:Pay group not available in "pay group" field  for Query # 6 PCARD_PAYGROUP_CH </t>
+  </si>
+  <si>
+    <t>BE_6:Voucher not available in Peoplesoft</t>
+  </si>
+  <si>
+    <t>BE_7:Voucher already on hold</t>
+  </si>
+  <si>
+    <t>BE_8:Location does not contain IA or I/A</t>
+  </si>
+  <si>
+    <t>LocalFolder</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_LocalFolder</t>
+  </si>
+  <si>
+    <t>Full path of the local folder where files will be processed</t>
+  </si>
+  <si>
+    <t>PeoplesoftCredentialAssetFolder</t>
+  </si>
+  <si>
+    <t>This is the credential asset folder</t>
+  </si>
+  <si>
+    <t>BE_9</t>
+  </si>
+  <si>
+    <t>BE_9:Location not found in search</t>
   </si>
   <si>
     <r>
       <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
-Process Monitor refresh failed because the duration dropdown did not contain the value that was configured. Please complete today's pay cycle manually; bot will resume next business day.&lt;br&gt;&lt;br&gt;
+The drop down 'Other is unavailable in dropdown option Hold Reason. Please perform the case manually&lt;br&gt;&lt;br&gt;
 </t>
     </r>
     <r>
@@ -413,234 +545,82 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Please correct the duration dropdown value prior to the next Bot run&lt;br&gt;&lt;br&gt;
+      <t xml:space="preserve">Please confirm that the login credentials are valid / updated prior to the next Bot run&lt;br&gt;&lt;br&gt;
 Thanks,&lt;br&gt;
 Automation Team
 </t>
     </r>
   </si>
   <si>
-    <t>SE_4</t>
-  </si>
-  <si>
-    <t>SE_4: Navigation to Process Monitor failed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
-Navigation to Process Monitor failed as the application was not responsive. Please complete today's pay cycle manually; bot will resume next business day.&lt;br&gt;&lt;br&gt;
+    <t>SE_5</t>
+  </si>
+  <si>
+    <t>SE_5:Other dropdown unavailable in Hold reason</t>
+  </si>
+  <si>
+    <t>HoldReason</t>
+  </si>
+  <si>
+    <t>P001_090_PayCycleQueries_HoldReason</t>
+  </si>
+  <si>
+    <t>Option for hold reason</t>
+  </si>
+  <si>
+    <t>PROD/P001_090_PayCycleQueries</t>
+  </si>
+  <si>
+    <t>PROD</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>SE: Unexpected error occurred - {Exception Details}</t>
+  </si>
+  <si>
+    <t>Unexpected error occurred in {Process Name} Process</t>
+  </si>
+  <si>
+    <t>Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
+The process faced an unexpected error. The error details are as follows&lt;br&gt;&lt;br&gt;
+&lt;u&gt;Error Details:&lt;/u&gt; {Exception Details}&lt;br&gt;&lt;br&gt;
 Thanks,&lt;br&gt;
-Automation Team
-</t>
-  </si>
-  <si>
-    <t>BE_1</t>
-  </si>
-  <si>
-    <t>BE_1: Unable to view queries in process monitor</t>
-  </si>
-  <si>
-    <t>Business Exception</t>
-  </si>
-  <si>
-    <t>Queries unavailable in Peoplesoft</t>
-  </si>
-  <si>
-    <t>Hi Statewide Accounting Team,&lt;br&gt;&lt;br&gt;
-The queries are inaccessible on the homepage. Kindly perform the pay cycle queries manually, and the bot will resume this process during the next run.&lt;br&gt;&lt;br&gt;
-Thanks,&lt;br&gt;
-Automation Team&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>BE_2</t>
-  </si>
-  <si>
-    <t>BE_2: Attachment not available</t>
-  </si>
-  <si>
-    <t>Bot :
-Make note of it summary report</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>BE_3</t>
-  </si>
-  <si>
-    <t>BE_3: Records not available in excel</t>
-  </si>
-  <si>
-    <t>BE_4</t>
-  </si>
-  <si>
-    <t>BE_4:Vouchers not available after filters and validation</t>
-  </si>
-  <si>
-    <t>BE_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pay group not available in "pay group" field  for Query # 6 PCARD_PAYGROUP_CH </t>
-  </si>
-  <si>
-    <t>SummaryPath</t>
-  </si>
-  <si>
-    <t>P001_090_PayCycleQueries_SummaryPath</t>
-  </si>
-  <si>
-    <t>BE_6</t>
-  </si>
-  <si>
-    <t>Voucher not available in Peoplesoft</t>
-  </si>
-  <si>
-    <t>SE_5</t>
-  </si>
-  <si>
-    <t>Location details not found in Add/Update Voucher page in Peoplesoft</t>
-  </si>
-  <si>
-    <t>BE_7</t>
-  </si>
-  <si>
-    <t>Voucher already on hold</t>
-  </si>
-  <si>
-    <t>BotControllerEmailID</t>
-  </si>
-  <si>
-    <t>P001_090_PayCycleQueries_BotControllerEmailID</t>
-  </si>
-  <si>
-    <t>The email IDs separated by comma for Bot controllers</t>
-  </si>
-  <si>
-    <t>BusinessEmailID</t>
-  </si>
-  <si>
-    <t>P001_090_PayCycleQueries_BusinessEmailID</t>
-  </si>
-  <si>
-    <t>The email IDs separated by comma for Business team</t>
-  </si>
-  <si>
-    <t>BotEmailID</t>
-  </si>
-  <si>
-    <t>P001_090_PayCycleQueries_BotEmailID</t>
-  </si>
-  <si>
-    <t>The email ID of the service account</t>
-  </si>
-  <si>
-    <t>DatetimeFormat</t>
-  </si>
-  <si>
-    <t>P001_090_PayCycleQueries_ProcessMonitorDatetimeFormat</t>
-  </si>
-  <si>
-    <t>The format of the date in process monitor to validate the run time of each instance</t>
-  </si>
-  <si>
-    <t>MorningStartTime</t>
-  </si>
-  <si>
-    <t>P001_090_PayCycleQueries_MorningRun_StartTime</t>
-  </si>
-  <si>
-    <t>Date time for Morning run</t>
-  </si>
-  <si>
-    <t>MorningEndTime</t>
-  </si>
-  <si>
-    <t>P001_090_PayCycleQueries_MorningRun_EndTime</t>
-  </si>
-  <si>
-    <t>NoonStartTime</t>
-  </si>
-  <si>
-    <t>P001_090_PayCycleQueries_NoonRun_StartTime</t>
-  </si>
-  <si>
-    <t>Date time for Noon run</t>
-  </si>
-  <si>
-    <t>NoonEndTime</t>
-  </si>
-  <si>
-    <t>P001_090_PayCycleQueries_NoonRun_EndTime</t>
-  </si>
-  <si>
-    <t>EveningStartTime</t>
-  </si>
-  <si>
-    <t>P001_090_PayCycleQueries_EveningRun_StartTime</t>
-  </si>
-  <si>
-    <t>Date time for Evening run</t>
-  </si>
-  <si>
-    <t>EveningEndTime</t>
-  </si>
-  <si>
-    <t>P001_090_PayCycleQueries_EveningRun_EndTime</t>
-  </si>
-  <si>
-    <t>StartEndTimeFormat</t>
-  </si>
-  <si>
-    <t>MM-dd-yyyy h:mmtt</t>
-  </si>
-  <si>
-    <t>The format used to parse time from assets</t>
-  </si>
-  <si>
-    <t>AssetFolder</t>
-  </si>
-  <si>
-    <t>TenantID</t>
-  </si>
-  <si>
-    <t>Shared_O365TenantID</t>
-  </si>
-  <si>
-    <t>Name of the Tenant ID Asset</t>
-  </si>
-  <si>
-    <t>AppID</t>
-  </si>
-  <si>
-    <t>Shared_O365ApplicationID</t>
-  </si>
-  <si>
-    <t>Name of the App ID Asset</t>
-  </si>
-  <si>
-    <t>AppSecret</t>
-  </si>
-  <si>
-    <t>Shared_O365ApplicationSecret</t>
-  </si>
-  <si>
-    <t>Name of the App Secret Asset</t>
-  </si>
-  <si>
-    <t>BE_8</t>
-  </si>
-  <si>
-    <t>Location does not contain IA or I/A</t>
+Automation Team</t>
+  </si>
+  <si>
+    <t>PeopleSoft application unavailable in {Process Name} Process</t>
+  </si>
+  <si>
+    <t>PeopleSoft login failed in {Process Name} Process</t>
+  </si>
+  <si>
+    <t>Other dropdown unavailable in Hold reason in {Process Name} Process</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -763,56 +743,59 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -833,9 +816,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -873,7 +856,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -979,7 +962,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1121,7 +1104,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1129,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z989"/>
+  <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1182,7 +1165,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -1193,7 +1176,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -1205,7 +1188,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -1216,70 +1199,80 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>161</v>
-      </c>
-      <c r="B9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C9" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
-        <v>164</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-    </row>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>167</v>
+        <v>128</v>
+      </c>
+      <c r="B12" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>168</v>
-      </c>
-      <c r="B13" t="s">
-        <v>169</v>
+        <v>129</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>170</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>132</v>
       </c>
       <c r="B14" t="s">
-        <v>172</v>
+        <v>133</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -2254,8 +2247,9 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
+    <row r="990" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="6"/>
+  <phoneticPr fontId="8"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3419,7 +3413,7 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="6"/>
+  <phoneticPr fontId="8"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3429,7 +3423,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C2" sqref="C2:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3484,263 +3478,289 @@
         <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>116</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>119</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>158</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>158</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
       <c r="B17" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>144</v>
+        <v>108</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1"/>
+      <c r="B21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>155</v>
+      </c>
+      <c r="B22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:4" ht="14.25" customHeight="1"/>
@@ -4714,7 +4734,7 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="6"/>
+  <phoneticPr fontId="8"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -4722,521 +4742,275 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E0E002E-D442-4416-9130-49903151FB44}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" customWidth="1"/>
-    <col min="7" max="7" width="49.42578125" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
-    <col min="12" max="12" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="49.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" customHeight="1">
+    <row r="1" spans="1:8" ht="18" customHeight="1">
       <c r="A1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="33" customHeight="1">
+      <c r="A2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="E2" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="F2" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="G2" s="9" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="120">
-      <c r="A2" s="7" t="s">
+      <c r="H2" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:8" ht="33" customHeight="1">
+      <c r="A3" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="39" customHeight="1">
+      <c r="A4" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="B4" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="D4" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="F4" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="39.75" customHeight="1">
+      <c r="A5" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="B5" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="F5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="39.75" customHeight="1">
+      <c r="A6" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45">
+      <c r="A7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="L2" s="7"/>
-    </row>
-    <row r="3" spans="1:12" ht="120">
-      <c r="A3" s="8" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="F7" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="30">
+      <c r="A8" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="B8" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="K3" s="10" t="s">
+      <c r="B9" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="195">
-      <c r="A4" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="K4" s="10" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" ht="30">
+      <c r="A10" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="225">
-      <c r="A5" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="K5" s="10" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" ht="30">
+      <c r="A11" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="L5" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="150">
-      <c r="A6" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="45">
-      <c r="A7" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="1:12" ht="135">
-      <c r="A8" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="45">
-      <c r="A9" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-    </row>
-    <row r="10" spans="1:12" ht="45">
-      <c r="A10" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="1:12" ht="45">
-      <c r="A11" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-    </row>
-    <row r="12" spans="1:12" ht="45">
-      <c r="A12" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:12" ht="45">
-      <c r="A13" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-    </row>
-    <row r="14" spans="1:12" ht="45">
-      <c r="A14" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-    </row>
-    <row r="15" spans="1:12" ht="45">
-      <c r="A15" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reverted back to logic of using process end dat to fetch queue items for summary report
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55648C\Documents\SOK_GIT\P0001_090_PayCyleQueries_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0125E2-78A0-4354-A90A-43757FD30101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E47FB53-7768-4463-AA8E-A2434A8F04E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,12 +18,25 @@
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
     <sheet name="Email" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="167">
   <si>
     <t>Name</t>
   </si>
@@ -591,10 +604,10 @@
 Automation Team</t>
   </si>
   <si>
-    <t>PROD/P001_090_PayCycleQueries</t>
-  </si>
-  <si>
-    <t>PROD</t>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>DEV</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1127,7 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1174,8 +1187,9 @@
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>165</v>
+      <c r="B3" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -1211,8 +1225,9 @@
       <c r="A8" t="s">
         <v>147</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>165</v>
+      <c r="B8" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>148</v>
@@ -1235,8 +1250,9 @@
       <c r="A12" t="s">
         <v>127</v>
       </c>
-      <c r="B12" t="s">
-        <v>166</v>
+      <c r="B12" t="str">
+        <f>Constants!$B$18</f>
+        <v>DEV</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -2259,7 +2275,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2440,7 +2456,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" t="s">
+        <v>166</v>
+      </c>
+    </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3422,7 +3445,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C22"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3476,8 +3499,9 @@
       <c r="B2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>165</v>
+      <c r="C2" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>68</v>
@@ -3490,8 +3514,9 @@
       <c r="B3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>165</v>
+      <c r="C3" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>69</v>
@@ -3504,8 +3529,9 @@
       <c r="B4" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>165</v>
+      <c r="C4" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>111</v>
@@ -3518,8 +3544,9 @@
       <c r="B5" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>165</v>
+      <c r="C5" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>111</v>
@@ -3532,8 +3559,9 @@
       <c r="B6" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>165</v>
+      <c r="C6" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>116</v>
@@ -3546,8 +3574,9 @@
       <c r="B7" t="s">
         <v>118</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>165</v>
+      <c r="C7" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>116</v>
@@ -3560,8 +3589,9 @@
       <c r="B8" t="s">
         <v>120</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>165</v>
+      <c r="C8" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>121</v>
@@ -3574,8 +3604,9 @@
       <c r="B9" t="s">
         <v>123</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>165</v>
+      <c r="C9" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>121</v>
@@ -3588,8 +3619,9 @@
       <c r="B10" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>165</v>
+      <c r="C10" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>67</v>
@@ -3602,8 +3634,9 @@
       <c r="B11" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>165</v>
+      <c r="C11" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>66</v>
@@ -3616,8 +3649,9 @@
       <c r="B12" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>165</v>
+      <c r="C12" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>65</v>
@@ -3630,8 +3664,9 @@
       <c r="B13" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>165</v>
+      <c r="C13" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>64</v>
@@ -3644,8 +3679,9 @@
       <c r="B14" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>165</v>
+      <c r="C14" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>63</v>
@@ -3658,8 +3694,9 @@
       <c r="B15" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>165</v>
+      <c r="C15" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>62</v>
@@ -3672,8 +3709,9 @@
       <c r="B16" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>165</v>
+      <c r="C16" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
@@ -3683,8 +3721,9 @@
       <c r="B17" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>165</v>
+      <c r="C17" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>99</v>
@@ -3697,8 +3736,9 @@
       <c r="B18" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>165</v>
+      <c r="C18" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>102</v>
@@ -3711,8 +3751,9 @@
       <c r="B19" t="s">
         <v>104</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>165</v>
+      <c r="C19" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>105</v>
@@ -3725,8 +3766,9 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>165</v>
+      <c r="C20" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>108</v>
@@ -3739,8 +3781,9 @@
       <c r="B21" t="s">
         <v>145</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>165</v>
+      <c r="C21" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>146</v>
@@ -3753,8 +3796,9 @@
       <c r="B22" t="s">
         <v>155</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>165</v>
+      <c r="C22" s="2" t="str">
+        <f>_xlfn.CONCAT(Constants!$B$18,"/P001_090_PayCycleQueries")</f>
+        <v>DEV/P001_090_PayCycleQueries</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>156</v>

</xml_diff>

<commit_message>
Added logic to send SE to bot controller and set the voucher column in Summary report to Text
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55648C\Documents\SOK_GIT\P0001_090_PayCyleQueries_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4EF621-D3D2-4BB8-877A-2D0DF7A2B3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53AEE00-29CE-41ED-A1A3-074983DEAB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="167">
   <si>
     <t>Name</t>
   </si>
@@ -4788,7 +4788,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4871,11 +4871,9 @@
         <v>82</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="H3" s="9" t="s">
         <v>84</v>
       </c>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" ht="39" customHeight="1">
       <c r="A4" s="7" t="s">

</xml_diff>